<commit_message>
Se agrega CP0003 y las pages SucursalesyCajeros y Eminent
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/Data.xlsx
+++ b/src/test/resources/datos/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorena.Bocian\IdeaProjects\TrabajoPOM_Bocian\src\test\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0222AB0-D7FD-41CD-A58D-9C2BA683486B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6A8D12-E48A-4948-AF5A-8DD6D07909E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18300" windowHeight="6510" xr2:uid="{1F9FC2AB-F047-4805-8DDD-B872CEDEB9A9}"/>
   </bookViews>
@@ -39,12 +39,6 @@
     <t>Dato3</t>
   </si>
   <si>
-    <t>CP003</t>
-  </si>
-  <si>
-    <t>Dato1CP3</t>
-  </si>
-  <si>
     <t>Dato2CP3</t>
   </si>
   <si>
@@ -130,6 +124,12 @@
   </si>
   <si>
     <t>div</t>
+  </si>
+  <si>
+    <t>Sucursales Exclusivas Éminent:</t>
+  </si>
+  <si>
+    <t>CP003_Eminent</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,119 +520,119 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1">
         <v>11223344</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>1234</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se Agrega el caso 0004
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/Data.xlsx
+++ b/src/test/resources/datos/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorena.Bocian\IdeaProjects\TrabajoPOM_Bocian\src\test\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6A8D12-E48A-4948-AF5A-8DD6D07909E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F33DCC1-8899-425B-ACDA-7E3DC60BE4F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18300" windowHeight="6510" xr2:uid="{1F9FC2AB-F047-4805-8DDD-B872CEDEB9A9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>CasosDePrueba</t>
   </si>
@@ -39,72 +39,18 @@
     <t>Dato3</t>
   </si>
   <si>
-    <t>Dato2CP3</t>
-  </si>
-  <si>
-    <t>Dato3CP3</t>
-  </si>
-  <si>
-    <t>CP004</t>
-  </si>
-  <si>
-    <t>Dato1CP4</t>
-  </si>
-  <si>
-    <t>Dato2CP4</t>
-  </si>
-  <si>
-    <t>Dato3CP4</t>
-  </si>
-  <si>
     <t>CP005</t>
   </si>
   <si>
-    <t>Dato1CP5</t>
-  </si>
-  <si>
-    <t>Dato2CP5</t>
-  </si>
-  <si>
-    <t>Dato3CP5</t>
-  </si>
-  <si>
     <t>CP006</t>
   </si>
   <si>
-    <t>Dato1CP6</t>
-  </si>
-  <si>
-    <t>Dato2CP6</t>
-  </si>
-  <si>
-    <t>Dato3CP6</t>
-  </si>
-  <si>
     <t>CP007</t>
   </si>
   <si>
-    <t>Dato1CP7</t>
-  </si>
-  <si>
-    <t>Dato2CP7</t>
-  </si>
-  <si>
-    <t>Dato3CP7</t>
-  </si>
-  <si>
     <t>CP008</t>
   </si>
   <si>
-    <t>Dato1CP8</t>
-  </si>
-  <si>
-    <t>Dato2CP8</t>
-  </si>
-  <si>
-    <t>Dato3CP8</t>
-  </si>
-  <si>
     <t>Dato4</t>
   </si>
   <si>
@@ -114,22 +60,31 @@
     <t>CP001_loginFallido</t>
   </si>
   <si>
-    <t>h5</t>
-  </si>
-  <si>
     <t>CP002_Busqueda</t>
   </si>
   <si>
     <t>asdfghjklñ</t>
   </si>
   <si>
-    <t>div</t>
-  </si>
-  <si>
     <t>Sucursales Exclusivas Éminent:</t>
   </si>
   <si>
     <t>CP003_Eminent</t>
+  </si>
+  <si>
+    <t>RIVADAVIA</t>
+  </si>
+  <si>
+    <t>CP004_Sucursal006</t>
+  </si>
+  <si>
+    <t>No es posible ingresar</t>
+  </si>
+  <si>
+    <t>No encontramos resultados para tu consulta. Te recomendamos usar frases cortas y palabras claves. Ej.: "caja de ahorro".</t>
+  </si>
+  <si>
+    <t>FLORES</t>
   </si>
 </sst>
 </file>
@@ -495,14 +450,14 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="24.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -520,119 +475,80 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>11223344</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>1234</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
+      <c r="D5" t="s">
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregan los test hasta el CP008
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/Data.xlsx
+++ b/src/test/resources/datos/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorena.Bocian\IdeaProjects\TrabajoPOM_Bocian\src\test\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F33DCC1-8899-425B-ACDA-7E3DC60BE4F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086F8872-268E-4B8A-A677-A725786AC000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18300" windowHeight="6510" xr2:uid="{1F9FC2AB-F047-4805-8DDD-B872CEDEB9A9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>CasosDePrueba</t>
   </si>
@@ -39,18 +39,6 @@
     <t>Dato3</t>
   </si>
   <si>
-    <t>CP005</t>
-  </si>
-  <si>
-    <t>CP006</t>
-  </si>
-  <si>
-    <t>CP007</t>
-  </si>
-  <si>
-    <t>CP008</t>
-  </si>
-  <si>
     <t>Dato4</t>
   </si>
   <si>
@@ -85,13 +73,41 @@
   </si>
   <si>
     <t>FLORES</t>
+  </si>
+  <si>
+    <t>CP005_Empresa</t>
+  </si>
+  <si>
+    <t>Centro Banca Empresas
+Asesoramiento especializado en todo el país, ese es nuestro centro.</t>
+  </si>
+  <si>
+    <t>CP006_Cajero</t>
+  </si>
+  <si>
+    <t>MORON</t>
+  </si>
+  <si>
+    <t>S1AGL065</t>
+  </si>
+  <si>
+    <t>CP007_Promociones</t>
+  </si>
+  <si>
+    <t>5 ELEMENTOS BAR</t>
+  </si>
+  <si>
+    <t>CP008_Promociones2</t>
+  </si>
+  <si>
+    <t>A LA PIPETUA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +122,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,9 +151,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -450,15 +476,16 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -475,80 +502,95 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>11223344</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>1234</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
       <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregan los ultimos cambios
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/Data.xlsx
+++ b/src/test/resources/datos/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorena.Bocian\IdeaProjects\TrabajoPOM_Bocian\src\test\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086F8872-268E-4B8A-A677-A725786AC000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4449712-09D3-4762-8061-026D84EF0CDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18300" windowHeight="6510" xr2:uid="{1F9FC2AB-F047-4805-8DDD-B872CEDEB9A9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>CasosDePrueba</t>
   </si>
@@ -94,13 +94,16 @@
     <t>CP007_Promociones</t>
   </si>
   <si>
-    <t>5 ELEMENTOS BAR</t>
-  </si>
-  <si>
     <t>CP008_Promociones2</t>
   </si>
   <si>
     <t>A LA PIPETUA</t>
+  </si>
+  <si>
+    <t>Computadora</t>
+  </si>
+  <si>
+    <t>No se han encontrado resultados para la búsqueda.</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,15 +585,18 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se suben los cambios del dia 31-08
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/Data.xlsx
+++ b/src/test/resources/datos/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorena.Bocian\IdeaProjects\TrabajoPOM_Bocian\src\test\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4449712-09D3-4762-8061-026D84EF0CDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA324529-0E7C-4B89-A449-3F0C8B0FB18D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18300" windowHeight="6510" xr2:uid="{1F9FC2AB-F047-4805-8DDD-B872CEDEB9A9}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>MORON</t>
   </si>
   <si>
-    <t>S1AGL065</t>
-  </si>
-  <si>
     <t>CP007_Promociones</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>No se han encontrado resultados para la búsqueda.</t>
+  </si>
+  <si>
+    <t>NUESTRA SRA.DEL BUEN VIAJE 739</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,26 +577,26 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>